<commit_message>
Tracking vis code update and other docs
</commit_message>
<xml_diff>
--- a/key-documents/R-chunks-chapter-codes.xlsx
+++ b/key-documents/R-chunks-chapter-codes.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://birdlife-my.sharepoint.com/personal/jonathan_handley_birdlife_org/Documents/JonoHandley_BirdLife/PROJECTS/Marine Toolkit/GitHub_MarineToolkit/MarMeCo-Toolkit-R-Beta/key-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABDACC10484D015C6DC65ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BA5C01A-6572-4693-9CA2-A367989E560A}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABDACC10484D015C6DC65ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83D0E806-0D7F-4A9E-9BF7-B7A5E6C84EA9}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Theme</t>
   </si>
@@ -49,6 +60,45 @@
   </si>
   <si>
     <t>Code-chunk-code-leading-abbreviation</t>
+  </si>
+  <si>
+    <t>Tracking data visualisation</t>
+  </si>
+  <si>
+    <t>rmd file name</t>
+  </si>
+  <si>
+    <t>03-TrackingData-Visualisation</t>
+  </si>
+  <si>
+    <t>track-vis</t>
+  </si>
+  <si>
+    <t>introduction</t>
+  </si>
+  <si>
+    <t>swe1</t>
+  </si>
+  <si>
+    <t>swe2</t>
+  </si>
+  <si>
+    <t>swe3</t>
+  </si>
+  <si>
+    <t>single colony</t>
+  </si>
+  <si>
+    <t>multiple colonies</t>
+  </si>
+  <si>
+    <t>background raster single</t>
+  </si>
+  <si>
+    <t>background raster multi</t>
+  </si>
+  <si>
+    <t>swe4</t>
   </si>
 </sst>
 </file>
@@ -101,6 +151,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,20 +420,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,24 +447,73 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>